<commit_message>
modified graphs to be black, to match theme of paper, finished conformance testing gathering of data, tweaked certain aspects of shor's, renamed github repo research
</commit_message>
<xml_diff>
--- a/Paper Figures/Conformance Testing/QKD results.xlsx
+++ b/Paper Figures/Conformance Testing/QKD results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Work\Quantum-Algorithm-Implementations\Paper Figures\Conformance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD0E550-05E6-4B6A-9C68-836D6934C135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29FE313-0FFD-49B5-86CA-C9B06C3B9768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-4755" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,235 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Qiskit</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="53">
+  <si>
+    <t>Quantum Key Distribution</t>
+  </si>
+  <si>
+    <t>Qiskit encode message</t>
+  </si>
+  <si>
+    <t>alice bits     = 1010101011110000</t>
+  </si>
+  <si>
+    <t>MeasureZ = 1000101111111000</t>
+  </si>
+  <si>
+    <t>MeasureX = 1010110010110000</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">alice bases = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>001110011010101</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>alice bits     = 1111111100000000</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">alice bases = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111111111111111</t>
+    </r>
+  </si>
+  <si>
+    <t>MeasureZ = 1101111110001101</t>
+  </si>
+  <si>
+    <t>MeasureX = 1111111100000000</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">alice bases = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0000000000000000</t>
+    </r>
+  </si>
+  <si>
+    <t>MeasureZ = 1111111100000000</t>
+  </si>
+  <si>
+    <t>MeasureX = 0111000011110100</t>
+  </si>
+  <si>
+    <t>Qiskit measure message</t>
+  </si>
+  <si>
+    <t>|0010100011100001|</t>
+  </si>
+  <si>
+    <t>|1010101011110000|</t>
+  </si>
+  <si>
+    <t>|1001001111010010|</t>
+  </si>
+  <si>
+    <t>Base 0 = Z and Base 1 = X</t>
+  </si>
+  <si>
+    <t>Qiskit remove garbage</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">alice bases = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111000011110000</t>
+    </r>
+  </si>
+  <si>
+    <t>bob bases   = 0000111100001111</t>
+  </si>
+  <si>
+    <t>Alice key</t>
+  </si>
+  <si>
+    <t>Bob key</t>
+  </si>
+  <si>
+    <t>||</t>
+  </si>
+  <si>
+    <t>bob bases   = 1111000000001111</t>
+  </si>
+  <si>
+    <t>|11111111|</t>
+  </si>
+  <si>
+    <t>bob bases   = 0000000011111111</t>
+  </si>
+  <si>
+    <t>|11110000|</t>
+  </si>
+  <si>
+    <t>bob bases   = 1111000011110000</t>
+  </si>
+  <si>
+    <t>|1111111100000000|</t>
+  </si>
+  <si>
+    <t>bob bases = 0011100110101010</t>
+  </si>
+  <si>
+    <t>Measurement with bob bases</t>
+  </si>
+  <si>
+    <t>bob bases =  1111111111111111</t>
+  </si>
+  <si>
+    <t>bob bases =  0000000000000000</t>
+  </si>
+  <si>
+    <t>Cirq encode message</t>
+  </si>
+  <si>
+    <t>Cirq measure message</t>
+  </si>
+  <si>
+    <t>Cirq remove garbage</t>
+  </si>
+  <si>
+    <t>|1011001111111000|</t>
+  </si>
+  <si>
+    <t>|1110110010110100|</t>
+  </si>
+  <si>
+    <t>MeasureX = 1111010110111100</t>
+  </si>
+  <si>
+    <t>MeasureZ = 1111010110111100</t>
+  </si>
+  <si>
+    <t>MeasureZ = 1011001111111000</t>
+  </si>
+  <si>
+    <t>MeasureX = 1110110010110100</t>
+  </si>
+  <si>
+    <t>Q# encode message</t>
+  </si>
+  <si>
+    <t>Q#  measure message</t>
+  </si>
+  <si>
+    <t>Q# measure message</t>
+  </si>
+  <si>
+    <t>Q# remove garbage</t>
+  </si>
+  <si>
+    <t>|1001001001010010|</t>
+  </si>
+  <si>
+    <t>|0010111010100000|</t>
+  </si>
+  <si>
+    <t>MeasureX = 0000101000100110</t>
+  </si>
+  <si>
+    <t>MeasureZ = 1011110011111001</t>
+  </si>
+  <si>
+    <t>MeasureX = 1110111010110100</t>
+  </si>
+  <si>
+    <t>MeasureZ = 1001001111011010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -345,18 +561,839 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" t="s">
+        <v>46</v>
+      </c>
+      <c r="H44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G47" t="s">
+        <v>28</v>
+      </c>
+      <c r="H47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>19</v>
+      </c>
+      <c r="B94" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>24</v>
+      </c>
+      <c r="B95" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>19</v>
+      </c>
+      <c r="B100" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>19</v>
+      </c>
+      <c r="B106" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>28</v>
+      </c>
+      <c r="B107" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>